<commit_message>
[MAJOR] Canada common docs processed
</commit_message>
<xml_diff>
--- a/sample/csv/5645e_excel.xlsx
+++ b/sample/csv/5645e_excel.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-20.04\home\nik\visaland-visa-form-utility\sample\csv\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{A9B8A69D-41A5-44CE-B638-089732AF0C5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8534D05-A9AE-4638-947E-5DD34BE98B64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4650" yWindow="3375" windowWidth="21600" windowHeight="4860"/>
+    <workbookView xWindow="4650" yWindow="3375" windowWidth="21600" windowHeight="7050" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="5645e" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="198">
   <si>
     <t>xfa:datasets.@xmlns:xfa</t>
   </si>
@@ -70,12 +70,6 @@
     <t>p1.SecA.Sps.SpsAddress</t>
   </si>
   <si>
-    <t>p1.SecA.Sps.SpsOccupation</t>
-  </si>
-  <si>
-    <t>p1.SecA.Sps.SpsYes</t>
-  </si>
-  <si>
     <t>p1.SecA.Sps.SpsNo</t>
   </si>
   <si>
@@ -94,12 +88,6 @@
     <t>p1.SecA.Mo.MoAddress</t>
   </si>
   <si>
-    <t>p1.SecA.Mo.MoOccupation</t>
-  </si>
-  <si>
-    <t>p1.SecA.Mo.MoYes</t>
-  </si>
-  <si>
     <t>p1.SecA.Mo.MoNo</t>
   </si>
   <si>
@@ -118,12 +106,6 @@
     <t>p1.SecA.Fa.FaAddress</t>
   </si>
   <si>
-    <t>p1.SecA.Fa.FaOccupation</t>
-  </si>
-  <si>
-    <t>p1.SecA.Fa.FaYes</t>
-  </si>
-  <si>
     <t>p1.SecA.Fa.FaNo</t>
   </si>
   <si>
@@ -145,24 +127,12 @@
     <t>p1.SecB.Chd.[0].ChdMStatus</t>
   </si>
   <si>
-    <t>p1.SecB.Chd.[0].ChdRelationship</t>
-  </si>
-  <si>
     <t>p1.SecB.Chd.[0].ChdDOB</t>
   </si>
   <si>
     <t>p1.SecB.Chd.[0].ChdCOB</t>
   </si>
   <si>
-    <t>p1.SecB.Chd.[0].ChdAddress</t>
-  </si>
-  <si>
-    <t>p1.SecB.Chd.[0].ChdOccupation</t>
-  </si>
-  <si>
-    <t>p1.SecB.Chd.[0].ChdYes</t>
-  </si>
-  <si>
     <t>p1.SecB.Chd.[0].ChdNo</t>
   </si>
   <si>
@@ -608,12 +578,48 @@
   </si>
   <si>
     <t>keep onehot -&gt; change type to int</t>
+  </si>
+  <si>
+    <t>p1.SecA.Sps.SpsOcc</t>
+  </si>
+  <si>
+    <t>p1.SecA.Sps.SpsAccomp</t>
+  </si>
+  <si>
+    <t>isnt Spouse's martial = Applicant martial?</t>
+  </si>
+  <si>
+    <t>p1.SecA.Mo.MoOcc</t>
+  </si>
+  <si>
+    <t>p1.SecA.Mo.MoAccomp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">if you are old, no one cares about your 90 yo parent prob, and if you are young, then its already included as accompany </t>
+  </si>
+  <si>
+    <t>p1.SecA.Fa.FaOcc</t>
+  </si>
+  <si>
+    <t>p1.SecA.Fa.FaAccomp</t>
+  </si>
+  <si>
+    <t>p1.SecB.Chd.[0].ChdRel</t>
+  </si>
+  <si>
+    <t>p1.SecB.Chd.[0].ChdAddr</t>
+  </si>
+  <si>
+    <t>p1.SecB.Chd.[0].ChdOcc</t>
+  </si>
+  <si>
+    <t>p1.SecB.Chd.[0].ChdAccomp</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1113,17 +1119,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1478,11 +1484,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:EO18"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="U1" workbookViewId="0">
-      <selection activeCell="Y6" sqref="Y6"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="AN1" workbookViewId="0">
+      <selection activeCell="AN1" sqref="AN1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1540,396 +1546,396 @@
         <v>15</v>
       </c>
       <c r="Q1" t="s">
+        <v>186</v>
+      </c>
+      <c r="R1" t="s">
+        <v>187</v>
+      </c>
+      <c r="S1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" t="s">
+      <c r="T1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" t="s">
+      <c r="U1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" t="s">
+      <c r="V1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" t="s">
+      <c r="W1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" t="s">
+      <c r="X1" t="s">
         <v>21</v>
       </c>
-      <c r="W1" t="s">
+      <c r="Y1" t="s">
+        <v>189</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>190</v>
+      </c>
+      <c r="AA1" t="s">
         <v>22</v>
       </c>
-      <c r="X1" t="s">
+      <c r="AB1" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="AC1" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AD1" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AE1" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AF1" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AG1" t="s">
+        <v>192</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>193</v>
+      </c>
+      <c r="AI1" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AJ1" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AK1" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AL1" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AM1" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AN1" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AO1" t="s">
         <v>34</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AP1" t="s">
+        <v>194</v>
+      </c>
+      <c r="AQ1" t="s">
         <v>35</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AR1" t="s">
         <v>36</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AS1" t="s">
+        <v>195</v>
+      </c>
+      <c r="AT1" t="s">
+        <v>196</v>
+      </c>
+      <c r="AU1" t="s">
+        <v>197</v>
+      </c>
+      <c r="AV1" t="s">
         <v>37</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="AW1" t="s">
         <v>38</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="AX1" t="s">
         <v>39</v>
       </c>
-      <c r="AO1" t="s">
+      <c r="AY1" t="s">
         <v>40</v>
       </c>
-      <c r="AP1" t="s">
+      <c r="AZ1" t="s">
         <v>41</v>
       </c>
-      <c r="AQ1" t="s">
+      <c r="BA1" t="s">
         <v>42</v>
       </c>
-      <c r="AR1" t="s">
+      <c r="BB1" t="s">
         <v>43</v>
       </c>
-      <c r="AS1" t="s">
+      <c r="BC1" t="s">
         <v>44</v>
       </c>
-      <c r="AT1" t="s">
+      <c r="BD1" t="s">
         <v>45</v>
       </c>
-      <c r="AU1" t="s">
+      <c r="BE1" t="s">
         <v>46</v>
       </c>
-      <c r="AV1" t="s">
+      <c r="BF1" t="s">
         <v>47</v>
       </c>
-      <c r="AW1" t="s">
+      <c r="BG1" t="s">
         <v>48</v>
       </c>
-      <c r="AX1" t="s">
+      <c r="BH1" t="s">
         <v>49</v>
       </c>
-      <c r="AY1" t="s">
+      <c r="BI1" t="s">
         <v>50</v>
       </c>
-      <c r="AZ1" t="s">
+      <c r="BJ1" t="s">
         <v>51</v>
       </c>
-      <c r="BA1" t="s">
+      <c r="BK1" t="s">
         <v>52</v>
       </c>
-      <c r="BB1" t="s">
+      <c r="BL1" t="s">
         <v>53</v>
       </c>
-      <c r="BC1" t="s">
+      <c r="BM1" t="s">
         <v>54</v>
       </c>
-      <c r="BD1" t="s">
+      <c r="BN1" t="s">
         <v>55</v>
       </c>
-      <c r="BE1" t="s">
+      <c r="BO1" t="s">
         <v>56</v>
       </c>
-      <c r="BF1" t="s">
+      <c r="BP1" t="s">
         <v>57</v>
       </c>
-      <c r="BG1" t="s">
+      <c r="BQ1" t="s">
         <v>58</v>
       </c>
-      <c r="BH1" t="s">
+      <c r="BR1" t="s">
         <v>59</v>
       </c>
-      <c r="BI1" t="s">
+      <c r="BS1" t="s">
         <v>60</v>
       </c>
-      <c r="BJ1" t="s">
+      <c r="BT1" t="s">
         <v>61</v>
       </c>
-      <c r="BK1" t="s">
+      <c r="BU1" t="s">
         <v>62</v>
       </c>
-      <c r="BL1" t="s">
+      <c r="BV1" t="s">
         <v>63</v>
       </c>
-      <c r="BM1" t="s">
+      <c r="BW1" t="s">
         <v>64</v>
       </c>
-      <c r="BN1" t="s">
+      <c r="BX1" t="s">
         <v>65</v>
       </c>
-      <c r="BO1" t="s">
+      <c r="BY1" t="s">
         <v>66</v>
       </c>
-      <c r="BP1" t="s">
+      <c r="BZ1" t="s">
         <v>67</v>
       </c>
-      <c r="BQ1" t="s">
+      <c r="CA1" t="s">
         <v>68</v>
       </c>
-      <c r="BR1" t="s">
+      <c r="CB1" t="s">
         <v>69</v>
       </c>
-      <c r="BS1" t="s">
+      <c r="CC1" t="s">
         <v>70</v>
       </c>
-      <c r="BT1" t="s">
+      <c r="CD1" t="s">
         <v>71</v>
       </c>
-      <c r="BU1" t="s">
+      <c r="CE1" t="s">
         <v>72</v>
       </c>
-      <c r="BV1" t="s">
+      <c r="CF1" t="s">
         <v>73</v>
       </c>
-      <c r="BW1" t="s">
+      <c r="CG1" t="s">
         <v>74</v>
       </c>
-      <c r="BX1" t="s">
+      <c r="CH1" t="s">
         <v>75</v>
       </c>
-      <c r="BY1" t="s">
+      <c r="CI1" t="s">
         <v>76</v>
       </c>
-      <c r="BZ1" t="s">
+      <c r="CJ1" t="s">
         <v>77</v>
       </c>
-      <c r="CA1" t="s">
+      <c r="CK1" t="s">
         <v>78</v>
       </c>
-      <c r="CB1" t="s">
+      <c r="CL1" t="s">
         <v>79</v>
       </c>
-      <c r="CC1" t="s">
+      <c r="CM1" t="s">
         <v>80</v>
       </c>
-      <c r="CD1" t="s">
+      <c r="CN1" t="s">
         <v>81</v>
       </c>
-      <c r="CE1" t="s">
+      <c r="CO1" t="s">
         <v>82</v>
       </c>
-      <c r="CF1" t="s">
+      <c r="CP1" t="s">
         <v>83</v>
       </c>
-      <c r="CG1" t="s">
+      <c r="CQ1" t="s">
         <v>84</v>
       </c>
-      <c r="CH1" t="s">
+      <c r="CR1" t="s">
         <v>85</v>
       </c>
-      <c r="CI1" t="s">
+      <c r="CS1" t="s">
         <v>86</v>
       </c>
-      <c r="CJ1" t="s">
+      <c r="CT1" t="s">
         <v>87</v>
       </c>
-      <c r="CK1" t="s">
+      <c r="CU1" t="s">
         <v>88</v>
       </c>
-      <c r="CL1" t="s">
+      <c r="CV1" t="s">
         <v>89</v>
       </c>
-      <c r="CM1" t="s">
+      <c r="CW1" t="s">
         <v>90</v>
       </c>
-      <c r="CN1" t="s">
+      <c r="CX1" t="s">
         <v>91</v>
       </c>
-      <c r="CO1" t="s">
+      <c r="CY1" t="s">
         <v>92</v>
       </c>
-      <c r="CP1" t="s">
+      <c r="CZ1" t="s">
         <v>93</v>
       </c>
-      <c r="CQ1" t="s">
+      <c r="DA1" t="s">
         <v>94</v>
       </c>
-      <c r="CR1" t="s">
+      <c r="DB1" t="s">
         <v>95</v>
       </c>
-      <c r="CS1" t="s">
+      <c r="DC1" t="s">
         <v>96</v>
       </c>
-      <c r="CT1" t="s">
+      <c r="DD1" t="s">
         <v>97</v>
       </c>
-      <c r="CU1" t="s">
+      <c r="DE1" t="s">
         <v>98</v>
       </c>
-      <c r="CV1" t="s">
+      <c r="DF1" t="s">
         <v>99</v>
       </c>
-      <c r="CW1" t="s">
+      <c r="DG1" t="s">
         <v>100</v>
       </c>
-      <c r="CX1" t="s">
+      <c r="DH1" t="s">
         <v>101</v>
       </c>
-      <c r="CY1" t="s">
+      <c r="DI1" t="s">
         <v>102</v>
       </c>
-      <c r="CZ1" t="s">
+      <c r="DJ1" t="s">
         <v>103</v>
       </c>
-      <c r="DA1" t="s">
+      <c r="DK1" t="s">
         <v>104</v>
       </c>
-      <c r="DB1" t="s">
+      <c r="DL1" t="s">
         <v>105</v>
       </c>
-      <c r="DC1" t="s">
+      <c r="DM1" t="s">
         <v>106</v>
       </c>
-      <c r="DD1" t="s">
+      <c r="DN1" t="s">
         <v>107</v>
       </c>
-      <c r="DE1" t="s">
+      <c r="DO1" t="s">
         <v>108</v>
       </c>
-      <c r="DF1" t="s">
+      <c r="DP1" t="s">
         <v>109</v>
       </c>
-      <c r="DG1" t="s">
+      <c r="DQ1" t="s">
         <v>110</v>
       </c>
-      <c r="DH1" t="s">
+      <c r="DR1" t="s">
         <v>111</v>
       </c>
-      <c r="DI1" t="s">
+      <c r="DS1" t="s">
         <v>112</v>
       </c>
-      <c r="DJ1" t="s">
+      <c r="DT1" t="s">
         <v>113</v>
       </c>
-      <c r="DK1" t="s">
+      <c r="DU1" t="s">
         <v>114</v>
       </c>
-      <c r="DL1" t="s">
+      <c r="DV1" t="s">
         <v>115</v>
       </c>
-      <c r="DM1" t="s">
+      <c r="DW1" t="s">
         <v>116</v>
       </c>
-      <c r="DN1" t="s">
+      <c r="DX1" t="s">
         <v>117</v>
       </c>
-      <c r="DO1" t="s">
+      <c r="DY1" t="s">
         <v>118</v>
       </c>
-      <c r="DP1" t="s">
+      <c r="DZ1" t="s">
         <v>119</v>
       </c>
-      <c r="DQ1" t="s">
+      <c r="EA1" t="s">
         <v>120</v>
       </c>
-      <c r="DR1" t="s">
+      <c r="EB1" t="s">
         <v>121</v>
       </c>
-      <c r="DS1" t="s">
+      <c r="EC1" t="s">
         <v>122</v>
       </c>
-      <c r="DT1" t="s">
+      <c r="ED1" t="s">
         <v>123</v>
       </c>
-      <c r="DU1" t="s">
+      <c r="EE1" t="s">
         <v>124</v>
       </c>
-      <c r="DV1" t="s">
+      <c r="EF1" t="s">
         <v>125</v>
       </c>
-      <c r="DW1" t="s">
+      <c r="EG1" t="s">
         <v>126</v>
       </c>
-      <c r="DX1" t="s">
+      <c r="EH1" t="s">
         <v>127</v>
       </c>
-      <c r="DY1" t="s">
+      <c r="EI1" t="s">
         <v>128</v>
       </c>
-      <c r="DZ1" t="s">
+      <c r="EJ1" t="s">
         <v>129</v>
       </c>
-      <c r="EA1" t="s">
+      <c r="EK1" t="s">
         <v>130</v>
       </c>
-      <c r="EB1" t="s">
+      <c r="EL1" t="s">
         <v>131</v>
       </c>
-      <c r="EC1" t="s">
+      <c r="EM1" t="s">
         <v>132</v>
       </c>
-      <c r="ED1" t="s">
+      <c r="EN1" t="s">
         <v>133</v>
       </c>
-      <c r="EE1" t="s">
+      <c r="EO1" t="s">
         <v>134</v>
-      </c>
-      <c r="EF1" t="s">
-        <v>135</v>
-      </c>
-      <c r="EG1" t="s">
-        <v>136</v>
-      </c>
-      <c r="EH1" t="s">
-        <v>137</v>
-      </c>
-      <c r="EI1" t="s">
-        <v>138</v>
-      </c>
-      <c r="EJ1" t="s">
-        <v>139</v>
-      </c>
-      <c r="EK1" t="s">
-        <v>140</v>
-      </c>
-      <c r="EL1" t="s">
-        <v>141</v>
-      </c>
-      <c r="EM1" t="s">
-        <v>142</v>
-      </c>
-      <c r="EN1" t="s">
-        <v>143</v>
-      </c>
-      <c r="EO1" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="2" spans="1:145" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -1944,40 +1950,40 @@
         <v>0</v>
       </c>
       <c r="F2" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
       <c r="G2" t="s">
-        <v>147</v>
+        <v>137</v>
       </c>
       <c r="H2" s="1">
         <v>23103</v>
       </c>
       <c r="I2" t="s">
-        <v>148</v>
+        <v>138</v>
       </c>
       <c r="J2" t="s">
-        <v>149</v>
+        <v>139</v>
       </c>
       <c r="K2" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="L2">
         <v>5</v>
       </c>
       <c r="M2" t="s">
-        <v>151</v>
+        <v>141</v>
       </c>
       <c r="N2" s="1">
         <v>21358</v>
       </c>
       <c r="O2" t="s">
-        <v>148</v>
+        <v>138</v>
       </c>
       <c r="P2" t="s">
-        <v>149</v>
+        <v>139</v>
       </c>
       <c r="Q2" t="s">
-        <v>152</v>
+        <v>142</v>
       </c>
       <c r="R2">
         <v>0</v>
@@ -1989,16 +1995,16 @@
         <v>5</v>
       </c>
       <c r="U2" t="s">
-        <v>153</v>
+        <v>143</v>
       </c>
       <c r="V2" s="1">
         <v>8620</v>
       </c>
       <c r="W2" t="s">
-        <v>148</v>
+        <v>138</v>
       </c>
       <c r="X2" t="s">
-        <v>154</v>
+        <v>144</v>
       </c>
       <c r="Z2">
         <v>0</v>
@@ -2007,16 +2013,16 @@
         <v>1</v>
       </c>
       <c r="AC2" t="s">
-        <v>155</v>
+        <v>145</v>
       </c>
       <c r="AD2" s="1">
         <v>7260</v>
       </c>
       <c r="AE2" t="s">
-        <v>148</v>
+        <v>138</v>
       </c>
       <c r="AF2" t="s">
-        <v>156</v>
+        <v>146</v>
       </c>
       <c r="AH2">
         <v>0</v>
@@ -2028,25 +2034,25 @@
         <v>43990</v>
       </c>
       <c r="AM2" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
       <c r="AN2" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="AO2">
         <v>5</v>
       </c>
       <c r="AP2" t="s">
-        <v>158</v>
+        <v>148</v>
       </c>
       <c r="AR2" t="s">
-        <v>148</v>
+        <v>138</v>
       </c>
       <c r="AS2" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="AT2" t="s">
-        <v>160</v>
+        <v>150</v>
       </c>
       <c r="AU2">
         <v>0</v>
@@ -2055,22 +2061,22 @@
         <v>1</v>
       </c>
       <c r="AW2" t="s">
-        <v>161</v>
+        <v>151</v>
       </c>
       <c r="AY2" t="s">
-        <v>158</v>
+        <v>148</v>
       </c>
       <c r="AZ2" s="1">
         <v>33535</v>
       </c>
       <c r="BA2" t="s">
-        <v>148</v>
+        <v>138</v>
       </c>
       <c r="BB2" t="s">
-        <v>149</v>
+        <v>139</v>
       </c>
       <c r="BC2" t="s">
-        <v>162</v>
+        <v>152</v>
       </c>
       <c r="BD2">
         <v>0</v>
@@ -2094,28 +2100,28 @@
         <v>43990</v>
       </c>
       <c r="BZ2" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
       <c r="CA2" t="s">
-        <v>163</v>
+        <v>153</v>
       </c>
       <c r="CB2">
         <v>5</v>
       </c>
       <c r="CC2" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
       <c r="CD2" s="1">
         <v>19559</v>
       </c>
       <c r="CE2" t="s">
-        <v>148</v>
+        <v>138</v>
       </c>
       <c r="CF2" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="CG2" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="CH2">
         <v>0</v>
@@ -2127,19 +2133,19 @@
         <v>5</v>
       </c>
       <c r="CK2" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
       <c r="CL2" s="1">
         <v>21996</v>
       </c>
       <c r="CM2" t="s">
-        <v>148</v>
+        <v>138</v>
       </c>
       <c r="CN2" t="s">
-        <v>167</v>
+        <v>157</v>
       </c>
       <c r="CO2" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="CP2">
         <v>0</v>
@@ -2148,28 +2154,28 @@
         <v>1</v>
       </c>
       <c r="CR2" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="CS2" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="CT2">
         <v>5</v>
       </c>
       <c r="CU2" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
       <c r="CV2" s="1">
         <v>24001</v>
       </c>
       <c r="CW2" t="s">
-        <v>148</v>
+        <v>138</v>
       </c>
       <c r="CX2" t="s">
-        <v>170</v>
+        <v>160</v>
       </c>
       <c r="CY2" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="CZ2">
         <v>0</v>
@@ -2178,25 +2184,25 @@
         <v>1</v>
       </c>
       <c r="DB2" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
       <c r="DC2">
         <v>7</v>
       </c>
       <c r="DD2" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
       <c r="DE2" s="1">
         <v>16427</v>
       </c>
       <c r="DF2" t="s">
-        <v>148</v>
+        <v>138</v>
       </c>
       <c r="DG2" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
       <c r="DH2" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="DI2">
         <v>0</v>
@@ -2205,25 +2211,25 @@
         <v>1</v>
       </c>
       <c r="DK2" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
       <c r="DL2">
         <v>7</v>
       </c>
       <c r="DM2" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
       <c r="DN2" s="1">
         <v>18102</v>
       </c>
       <c r="DO2" t="s">
-        <v>148</v>
+        <v>138</v>
       </c>
       <c r="DP2" t="s">
-        <v>175</v>
+        <v>165</v>
       </c>
       <c r="DQ2" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="DR2">
         <v>0</v>
@@ -2232,25 +2238,25 @@
         <v>1</v>
       </c>
       <c r="DT2" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
       <c r="DU2">
         <v>7</v>
       </c>
       <c r="DV2" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
       <c r="DW2" s="1">
         <v>18562</v>
       </c>
       <c r="DX2" t="s">
-        <v>148</v>
+        <v>138</v>
       </c>
       <c r="DY2" t="s">
-        <v>177</v>
+        <v>167</v>
       </c>
       <c r="DZ2" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="EA2">
         <v>0</v>
@@ -2259,25 +2265,25 @@
         <v>1</v>
       </c>
       <c r="EC2" t="s">
-        <v>178</v>
+        <v>168</v>
       </c>
       <c r="ED2">
         <v>3</v>
       </c>
       <c r="EE2" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
       <c r="EF2" s="1">
         <v>21043</v>
       </c>
       <c r="EG2" t="s">
-        <v>148</v>
+        <v>138</v>
       </c>
       <c r="EH2" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
       <c r="EI2" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="EJ2">
         <v>0</v>
@@ -2289,529 +2295,568 @@
         <v>43990</v>
       </c>
       <c r="EN2" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
       <c r="EO2" t="s">
-        <v>180</v>
+        <v>170</v>
       </c>
     </row>
     <row r="4" spans="1:145" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>195</v>
-      </c>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
+        <v>171</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
       <c r="F4" s="2" t="s">
-        <v>181</v>
+        <v>171</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>181</v>
+        <v>171</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>182</v>
+        <v>172</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>182</v>
+        <v>172</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>181</v>
+        <v>171</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>182</v>
+        <v>172</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>174</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="N4" s="5" t="s">
-        <v>183</v>
-      </c>
-      <c r="O4" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="N4" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="O4" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="P4" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="Q4" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="R4" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="S4" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="T4" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="U4" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="V4" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="W4" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="X4" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="Y4" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="Z4" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="AA4" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="AB4" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="AC4" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="AD4" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="AE4" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="AF4" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="AG4" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="AH4" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="AI4" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="AJ4" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="AK4" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="AL4" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="AM4" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="AN4" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="AO4" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="AP4" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="AQ4" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="AR4" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="AS4" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="AT4" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="AU4" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="AV4" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="AW4" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="AX4" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="AY4" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="AZ4" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="BA4" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="BB4" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="BC4" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="BD4" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="BE4" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="BF4" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="BG4" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="BH4" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="BI4" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="BJ4" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="BK4" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="BL4" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="BM4" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="BN4" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="BO4" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="BP4" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="BQ4" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="BR4" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="BS4" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="BT4" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="BU4" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="BV4" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="BW4" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="BX4" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="BY4" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="BZ4" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="CA4" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="CB4" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="CC4" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="CD4" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="CE4" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="CF4" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="CG4" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="CH4" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="CI4" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="CJ4" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="CK4" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="CL4" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="CM4" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="CN4" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="CO4" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="CP4" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="CQ4" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="CR4" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="CS4" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="CT4" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="CU4" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="CV4" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="CW4" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="CX4" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="CY4" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="CZ4" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="DA4" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="DB4" s="6" t="s">
         <v>184</v>
       </c>
-      <c r="P4" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="Q4" s="5" t="s">
-        <v>184</v>
-      </c>
-      <c r="R4" s="5" t="s">
-        <v>185</v>
-      </c>
-      <c r="S4" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="T4" s="5" t="s">
-        <v>184</v>
-      </c>
-      <c r="U4" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="V4" s="5" t="s">
-        <v>183</v>
-      </c>
-      <c r="W4" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="X4" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="Y4" s="5" t="s">
-        <v>184</v>
-      </c>
-      <c r="Z4" s="5" t="s">
-        <v>185</v>
-      </c>
-      <c r="AA4" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="AB4" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="AC4" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="AD4" s="5" t="s">
-        <v>183</v>
-      </c>
-      <c r="AE4" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="AF4" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="AG4" s="5" t="s">
-        <v>184</v>
-      </c>
-      <c r="AH4" s="5" t="s">
-        <v>185</v>
-      </c>
-      <c r="AI4" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="AK4" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="AL4" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="AM4" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="AN4" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="AO4" s="5" t="s">
-        <v>184</v>
-      </c>
-      <c r="AP4" s="5" t="s">
-        <v>185</v>
-      </c>
-      <c r="AQ4" s="5" t="s">
-        <v>183</v>
-      </c>
-      <c r="AR4" s="5" t="s">
-        <v>184</v>
-      </c>
-      <c r="AS4" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="AT4" s="5" t="s">
-        <v>184</v>
-      </c>
-      <c r="AU4" s="5" t="s">
-        <v>185</v>
-      </c>
-      <c r="AV4" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="AW4" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="AX4" s="5" t="s">
-        <v>184</v>
-      </c>
-      <c r="AY4" s="5" t="s">
-        <v>185</v>
-      </c>
-      <c r="AZ4" s="5" t="s">
-        <v>183</v>
-      </c>
-      <c r="BA4" s="5" t="s">
-        <v>184</v>
-      </c>
-      <c r="BB4" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="BC4" s="5" t="s">
-        <v>184</v>
-      </c>
-      <c r="BD4" s="5" t="s">
-        <v>185</v>
-      </c>
-      <c r="BE4" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="BF4" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="BG4" s="5" t="s">
-        <v>184</v>
-      </c>
-      <c r="BH4" s="5" t="s">
-        <v>185</v>
-      </c>
-      <c r="BI4" s="5" t="s">
-        <v>183</v>
-      </c>
-      <c r="BJ4" s="5" t="s">
-        <v>184</v>
-      </c>
-      <c r="BK4" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="BL4" s="5" t="s">
-        <v>184</v>
-      </c>
-      <c r="BM4" s="5" t="s">
-        <v>185</v>
-      </c>
-      <c r="BN4" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="BO4" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="BP4" s="5" t="s">
-        <v>184</v>
-      </c>
-      <c r="BQ4" s="5" t="s">
-        <v>185</v>
-      </c>
-      <c r="BR4" s="5" t="s">
-        <v>183</v>
-      </c>
-      <c r="BS4" s="5" t="s">
-        <v>184</v>
-      </c>
-      <c r="BT4" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="BU4" s="5" t="s">
-        <v>184</v>
-      </c>
-      <c r="BV4" s="5" t="s">
-        <v>185</v>
-      </c>
-      <c r="BW4" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="BX4" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="BY4" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="BZ4" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="CA4" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="CB4" s="5" t="s">
-        <v>184</v>
-      </c>
-      <c r="CC4" s="5" t="s">
-        <v>184</v>
-      </c>
-      <c r="CD4" s="5" t="s">
-        <v>183</v>
-      </c>
-      <c r="CE4" s="5" t="s">
-        <v>185</v>
-      </c>
-      <c r="CF4" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="CG4" s="5" t="s">
-        <v>184</v>
-      </c>
-      <c r="CH4" s="5" t="s">
-        <v>185</v>
-      </c>
-      <c r="CI4" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="CJ4" s="5" t="s">
-        <v>184</v>
-      </c>
-      <c r="CK4" s="5" t="s">
-        <v>184</v>
-      </c>
-      <c r="CL4" s="5" t="s">
-        <v>183</v>
-      </c>
-      <c r="CM4" s="5" t="s">
-        <v>185</v>
-      </c>
-      <c r="CN4" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="CO4" s="5" t="s">
-        <v>184</v>
-      </c>
-      <c r="CP4" s="5" t="s">
-        <v>185</v>
-      </c>
-      <c r="CQ4" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="CR4" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="CS4" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="CT4" s="5" t="s">
-        <v>184</v>
-      </c>
-      <c r="CU4" s="5" t="s">
-        <v>184</v>
-      </c>
-      <c r="CV4" s="5" t="s">
-        <v>183</v>
-      </c>
-      <c r="CW4" s="5" t="s">
-        <v>185</v>
-      </c>
-      <c r="CX4" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="CY4" s="5" t="s">
-        <v>184</v>
-      </c>
-      <c r="CZ4" s="5" t="s">
-        <v>185</v>
-      </c>
-      <c r="DA4" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="DB4" s="3" t="s">
-        <v>194</v>
-      </c>
       <c r="EL4" s="2" t="s">
-        <v>181</v>
+        <v>171</v>
       </c>
       <c r="EM4" s="2" t="s">
-        <v>181</v>
+        <v>171</v>
       </c>
       <c r="EN4" s="2" t="s">
-        <v>181</v>
+        <v>171</v>
       </c>
       <c r="EO4" s="2" t="s">
-        <v>181</v>
+        <v>171</v>
       </c>
     </row>
     <row r="5" spans="1:145" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>181</v>
+        <v>171</v>
       </c>
       <c r="F5" t="s">
-        <v>181</v>
+        <v>171</v>
       </c>
       <c r="H5" t="s">
-        <v>181</v>
+        <v>171</v>
       </c>
       <c r="I5" t="s">
-        <v>181</v>
+        <v>171</v>
       </c>
       <c r="K5" t="s">
-        <v>181</v>
-      </c>
-      <c r="V5" s="3"/>
+        <v>171</v>
+      </c>
+      <c r="T5" t="s">
+        <v>188</v>
+      </c>
+      <c r="V5" s="6"/>
+      <c r="AB5" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="AJ5" s="6" t="s">
+        <v>191</v>
+      </c>
       <c r="AK5" t="s">
-        <v>181</v>
+        <v>171</v>
       </c>
       <c r="AL5" t="s">
-        <v>181</v>
+        <v>171</v>
       </c>
       <c r="AM5" t="s">
-        <v>181</v>
+        <v>171</v>
       </c>
       <c r="BX5" t="s">
-        <v>181</v>
+        <v>171</v>
       </c>
       <c r="BY5" t="s">
-        <v>181</v>
+        <v>171</v>
       </c>
       <c r="BZ5" t="s">
-        <v>181</v>
-      </c>
-      <c r="DB5" s="3"/>
+        <v>171</v>
+      </c>
+      <c r="DB5" s="6"/>
       <c r="EL5" t="s">
-        <v>181</v>
+        <v>171</v>
       </c>
     </row>
     <row r="6" spans="1:145" x14ac:dyDescent="0.25">
-      <c r="V6" s="3"/>
-      <c r="W6" s="3" t="s">
-        <v>186</v>
-      </c>
-      <c r="AE6" s="3" t="s">
-        <v>186</v>
-      </c>
-      <c r="AO6" s="3" t="s">
-        <v>188</v>
-      </c>
-      <c r="AQ6" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="AR6" s="3" t="s">
-        <v>189</v>
-      </c>
-      <c r="AT6" s="3" t="s">
-        <v>190</v>
-      </c>
-      <c r="AX6" s="3" t="s">
-        <v>188</v>
-      </c>
-      <c r="AZ6" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="BA6" s="3" t="s">
-        <v>189</v>
-      </c>
-      <c r="BC6" s="3" t="s">
-        <v>190</v>
-      </c>
-      <c r="BG6" s="3" t="s">
-        <v>188</v>
-      </c>
-      <c r="BI6" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="BJ6" s="3" t="s">
-        <v>189</v>
-      </c>
-      <c r="BL6" s="3" t="s">
-        <v>190</v>
-      </c>
-      <c r="BP6" s="3" t="s">
-        <v>188</v>
-      </c>
-      <c r="BR6" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="BS6" s="3" t="s">
-        <v>189</v>
-      </c>
-      <c r="BU6" s="3" t="s">
-        <v>190</v>
-      </c>
-      <c r="CE6" s="3" t="s">
-        <v>192</v>
-      </c>
-      <c r="CM6" s="3" t="s">
-        <v>192</v>
-      </c>
-      <c r="CW6" s="3" t="s">
-        <v>192</v>
-      </c>
-      <c r="DB6" s="6" t="s">
-        <v>193</v>
+      <c r="V6" s="6"/>
+      <c r="W6" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="AB6" s="6"/>
+      <c r="AE6" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="AJ6" s="6"/>
+      <c r="AO6" s="6" t="s">
+        <v>178</v>
+      </c>
+      <c r="AQ6" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="AR6" s="6" t="s">
+        <v>179</v>
+      </c>
+      <c r="AT6" s="6" t="s">
+        <v>180</v>
+      </c>
+      <c r="AX6" s="6" t="s">
+        <v>178</v>
+      </c>
+      <c r="AZ6" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="BA6" s="6" t="s">
+        <v>179</v>
+      </c>
+      <c r="BC6" s="6" t="s">
+        <v>180</v>
+      </c>
+      <c r="BG6" s="6" t="s">
+        <v>178</v>
+      </c>
+      <c r="BI6" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="BJ6" s="6" t="s">
+        <v>179</v>
+      </c>
+      <c r="BL6" s="6" t="s">
+        <v>180</v>
+      </c>
+      <c r="BP6" s="6" t="s">
+        <v>178</v>
+      </c>
+      <c r="BR6" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="BS6" s="6" t="s">
+        <v>179</v>
+      </c>
+      <c r="BU6" s="6" t="s">
+        <v>180</v>
+      </c>
+      <c r="CE6" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="CM6" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="CW6" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="DB6" s="5" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="7" spans="1:145" x14ac:dyDescent="0.25">
-      <c r="V7" s="3"/>
-      <c r="W7" s="3"/>
-      <c r="AE7" s="3"/>
-      <c r="AO7" s="3"/>
-      <c r="AQ7" s="3"/>
-      <c r="AR7" s="3"/>
-      <c r="AT7" s="3"/>
-      <c r="AX7" s="3"/>
-      <c r="AZ7" s="3"/>
-      <c r="BA7" s="3"/>
-      <c r="BC7" s="3"/>
-      <c r="BG7" s="3"/>
-      <c r="BI7" s="3"/>
-      <c r="BJ7" s="3"/>
-      <c r="BL7" s="3"/>
-      <c r="BP7" s="3"/>
-      <c r="BR7" s="3"/>
-      <c r="BS7" s="3"/>
-      <c r="BU7" s="3"/>
-      <c r="CE7" s="3"/>
-      <c r="CM7" s="3"/>
-      <c r="CW7" s="3"/>
-      <c r="DB7" s="6"/>
+      <c r="V7" s="6"/>
+      <c r="W7" s="6"/>
+      <c r="AB7" s="6"/>
+      <c r="AE7" s="6"/>
+      <c r="AJ7" s="6"/>
+      <c r="AO7" s="6"/>
+      <c r="AQ7" s="6"/>
+      <c r="AR7" s="6"/>
+      <c r="AT7" s="6"/>
+      <c r="AX7" s="6"/>
+      <c r="AZ7" s="6"/>
+      <c r="BA7" s="6"/>
+      <c r="BC7" s="6"/>
+      <c r="BG7" s="6"/>
+      <c r="BI7" s="6"/>
+      <c r="BJ7" s="6"/>
+      <c r="BL7" s="6"/>
+      <c r="BP7" s="6"/>
+      <c r="BR7" s="6"/>
+      <c r="BS7" s="6"/>
+      <c r="BU7" s="6"/>
+      <c r="CE7" s="6"/>
+      <c r="CM7" s="6"/>
+      <c r="CW7" s="6"/>
+      <c r="DB7" s="5"/>
     </row>
     <row r="8" spans="1:145" x14ac:dyDescent="0.25">
-      <c r="V8" s="3"/>
-      <c r="W8" s="3"/>
-      <c r="AE8" s="3"/>
-      <c r="AO8" s="3"/>
-      <c r="AQ8" s="3"/>
-      <c r="AR8" s="3"/>
-      <c r="AT8" s="3"/>
-      <c r="AX8" s="3"/>
-      <c r="AZ8" s="3"/>
-      <c r="BA8" s="3"/>
-      <c r="BC8" s="3"/>
-      <c r="BG8" s="3"/>
-      <c r="BI8" s="3"/>
-      <c r="BJ8" s="3"/>
-      <c r="BL8" s="3"/>
-      <c r="BP8" s="3"/>
-      <c r="BR8" s="3"/>
-      <c r="BS8" s="3"/>
-      <c r="BU8" s="3"/>
-      <c r="CE8" s="3"/>
-      <c r="CM8" s="3"/>
-      <c r="CW8" s="3"/>
-      <c r="DB8" s="6"/>
+      <c r="V8" s="6"/>
+      <c r="W8" s="6"/>
+      <c r="AE8" s="6"/>
+      <c r="AO8" s="6"/>
+      <c r="AQ8" s="6"/>
+      <c r="AR8" s="6"/>
+      <c r="AT8" s="6"/>
+      <c r="AX8" s="6"/>
+      <c r="AZ8" s="6"/>
+      <c r="BA8" s="6"/>
+      <c r="BC8" s="6"/>
+      <c r="BG8" s="6"/>
+      <c r="BI8" s="6"/>
+      <c r="BJ8" s="6"/>
+      <c r="BL8" s="6"/>
+      <c r="BP8" s="6"/>
+      <c r="BR8" s="6"/>
+      <c r="BS8" s="6"/>
+      <c r="BU8" s="6"/>
+      <c r="CE8" s="6"/>
+      <c r="CM8" s="6"/>
+      <c r="CW8" s="6"/>
+      <c r="DB8" s="5"/>
     </row>
     <row r="9" spans="1:145" x14ac:dyDescent="0.25">
-      <c r="DB9" s="6"/>
+      <c r="DB9" s="5"/>
     </row>
     <row r="10" spans="1:145" x14ac:dyDescent="0.25">
-      <c r="CA10" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="DB10" s="6"/>
+      <c r="CA10" s="6" t="s">
+        <v>181</v>
+      </c>
+      <c r="DB10" s="5"/>
     </row>
     <row r="11" spans="1:145" x14ac:dyDescent="0.25">
-      <c r="CA11" s="3"/>
-      <c r="DB11" s="6"/>
+      <c r="CA11" s="6"/>
+      <c r="DB11" s="5"/>
     </row>
     <row r="12" spans="1:145" x14ac:dyDescent="0.25">
-      <c r="CA12" s="3"/>
-      <c r="DB12" s="6"/>
+      <c r="CA12" s="6"/>
+      <c r="DB12" s="5"/>
     </row>
     <row r="13" spans="1:145" x14ac:dyDescent="0.25">
-      <c r="CA13" s="3"/>
+      <c r="CA13" s="6"/>
     </row>
     <row r="14" spans="1:145" x14ac:dyDescent="0.25">
-      <c r="CA14" s="3"/>
-      <c r="DB14" s="7"/>
+      <c r="CA14" s="6"/>
+      <c r="DB14" s="4"/>
     </row>
     <row r="15" spans="1:145" x14ac:dyDescent="0.25">
-      <c r="DB15" s="7"/>
+      <c r="DB15" s="4"/>
     </row>
     <row r="16" spans="1:145" x14ac:dyDescent="0.25">
-      <c r="DB16" s="7"/>
+      <c r="DB16" s="4"/>
     </row>
     <row r="17" spans="106:106" x14ac:dyDescent="0.25">
-      <c r="DB17" s="7"/>
+      <c r="DB17" s="4"/>
     </row>
     <row r="18" spans="106:106" x14ac:dyDescent="0.25">
-      <c r="DB18" s="7"/>
+      <c r="DB18" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="26">
+  <mergeCells count="28">
+    <mergeCell ref="AQ6:AQ8"/>
+    <mergeCell ref="AB5:AB7"/>
+    <mergeCell ref="AJ5:AJ7"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="V5:V8"/>
+    <mergeCell ref="W6:W8"/>
+    <mergeCell ref="AE6:AE8"/>
+    <mergeCell ref="AO6:AO8"/>
+    <mergeCell ref="BR6:BR8"/>
+    <mergeCell ref="AR6:AR8"/>
+    <mergeCell ref="AT6:AT8"/>
+    <mergeCell ref="AX6:AX8"/>
+    <mergeCell ref="AZ6:AZ8"/>
+    <mergeCell ref="BA6:BA8"/>
+    <mergeCell ref="BC6:BC8"/>
+    <mergeCell ref="BG6:BG8"/>
+    <mergeCell ref="BI6:BI8"/>
+    <mergeCell ref="BJ6:BJ8"/>
+    <mergeCell ref="BL6:BL8"/>
+    <mergeCell ref="BP6:BP8"/>
     <mergeCell ref="DB6:DB12"/>
     <mergeCell ref="DB4:DB5"/>
     <mergeCell ref="BS6:BS8"/>
@@ -2820,24 +2865,6 @@
     <mergeCell ref="CE6:CE8"/>
     <mergeCell ref="CM6:CM8"/>
     <mergeCell ref="CW6:CW8"/>
-    <mergeCell ref="BG6:BG8"/>
-    <mergeCell ref="BI6:BI8"/>
-    <mergeCell ref="BJ6:BJ8"/>
-    <mergeCell ref="BL6:BL8"/>
-    <mergeCell ref="BP6:BP8"/>
-    <mergeCell ref="BR6:BR8"/>
-    <mergeCell ref="AR6:AR8"/>
-    <mergeCell ref="AT6:AT8"/>
-    <mergeCell ref="AX6:AX8"/>
-    <mergeCell ref="AZ6:AZ8"/>
-    <mergeCell ref="BA6:BA8"/>
-    <mergeCell ref="BC6:BC8"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="V5:V8"/>
-    <mergeCell ref="W6:W8"/>
-    <mergeCell ref="AE6:AE8"/>
-    <mergeCell ref="AO6:AO8"/>
-    <mergeCell ref="AQ6:AQ8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>